<commit_message>
modified:   run.py fixed styles , path , file save
</commit_message>
<xml_diff>
--- a/Excel O365 Automation Scenarios.xlsx
+++ b/Excel O365 Automation Scenarios.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBS\TopCoder\Infra Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Webapi123_part2\Excel-O365-Testcase-Automation-Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="595" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="595"/>
   </bookViews>
   <sheets>
     <sheet name="Excel O365" sheetId="1" r:id="rId1"/>
@@ -1581,7 +1581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2794,7 +2794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>

</xml_diff>